<commit_message>
Add sleep option for joint floatingip
</commit_message>
<xml_diff>
--- a/create-instance-list.xlsx
+++ b/create-instance-list.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="5820" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="インスタンスリスト" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>インスタンス名</t>
     <rPh sb="6" eb="7">
@@ -57,6 +57,10 @@
   </si>
   <si>
     <t>fuga</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>foo</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -435,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -488,6 +492,20 @@
         <v>6</v>
       </c>
       <c r="D3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>